<commit_message>
large corpora can be learned now!
</commit_message>
<xml_diff>
--- a/ProjectManagement/ProjektPlan.xlsx
+++ b/ProjectManagement/ProjektPlan.xlsx
@@ -3349,10 +3349,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ACA69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="U4" sqref="U4"/>
+      <selection pane="topRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -13713,19 +13713,19 @@
       </c>
       <c r="J23" s="80">
         <f>AVERAGE(J24:J28)</f>
-        <v>0.42499999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="K23" s="70">
         <f t="shared" ca="1" si="23"/>
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="L23" s="228">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M23" s="229">
         <f t="shared" si="24"/>
-        <v>42105</v>
+        <v>42107</v>
       </c>
       <c r="N23" s="206"/>
       <c r="O23" s="83"/>
@@ -13886,19 +13886,19 @@
         <v>42103</v>
       </c>
       <c r="J24" s="80">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="K24" s="70">
         <f t="shared" ca="1" si="23"/>
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="L24" s="228">
         <f t="shared" si="22"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M24" s="229">
         <f t="shared" si="24"/>
-        <v>42101</v>
+        <v>42102</v>
       </c>
       <c r="N24" s="206"/>
       <c r="O24" s="83"/>
@@ -14232,19 +14232,19 @@
         <v>42113</v>
       </c>
       <c r="J26" s="80">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K26" s="70">
         <f t="shared" ca="1" si="23"/>
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="L26" s="228">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26" s="229">
         <f t="shared" si="24"/>
-        <v>42108</v>
+        <v>42109</v>
       </c>
       <c r="N26" s="206"/>
       <c r="O26" s="83"/>

</xml_diff>